<commit_message>
Updated utility testing MultipleStatements
</commit_message>
<xml_diff>
--- a/Utilities/Table Excel Files/TblNames.xlsx
+++ b/Utilities/Table Excel Files/TblNames.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="TblNames"/>
   </sheets>
   <definedNames>
-    <definedName name="TblNames">'TblNames'!$A$1:$B$51</definedName>
+    <definedName name="TblNames">'TblNames'!$A$1:$B$52</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -365,7 +365,7 @@
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="0">
-        <v>548</v>
+        <v>710</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -375,7 +375,7 @@
     </row>
     <row outlineLevel="0" r="3">
       <c r="A3" s="0">
-        <v>549</v>
+        <v>711</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -385,7 +385,7 @@
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="0">
-        <v>550</v>
+        <v>712</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -395,7 +395,7 @@
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="0">
-        <v>551</v>
+        <v>713</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -405,7 +405,7 @@
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0">
-        <v>552</v>
+        <v>714</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -415,7 +415,7 @@
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0">
-        <v>553</v>
+        <v>715</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
@@ -425,7 +425,7 @@
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
-        <v>554</v>
+        <v>716</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
@@ -435,7 +435,7 @@
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
-        <v>555</v>
+        <v>717</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
@@ -445,7 +445,7 @@
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
-        <v>556</v>
+        <v>718</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
@@ -455,7 +455,7 @@
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
-        <v>557</v>
+        <v>719</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
@@ -465,7 +465,7 @@
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
-        <v>558</v>
+        <v>720</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
@@ -475,7 +475,7 @@
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="0">
-        <v>559</v>
+        <v>721</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
@@ -485,7 +485,7 @@
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="0">
-        <v>560</v>
+        <v>722</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="0">
-        <v>561</v>
+        <v>723</v>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
@@ -505,7 +505,7 @@
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="0">
-        <v>562</v>
+        <v>724</v>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
@@ -515,7 +515,7 @@
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="0">
-        <v>563</v>
+        <v>725</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="0">
-        <v>564</v>
+        <v>726</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
@@ -535,329 +535,339 @@
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="0">
-        <v>565</v>
+        <v>727</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>Tbl_DailyExposure</t>
+          <t>Tbl_CustomersList</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="0">
-        <v>566</v>
+        <v>728</v>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Deductions</t>
+          <t>Tbl_DailyExposure</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="0">
-        <v>567</v>
+        <v>729</v>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>Tbl_DepartmentNames</t>
+          <t>Tbl_Deductions</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="0">
-        <v>568</v>
+        <v>730</v>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>Tbl_DocumentsToBeErased</t>
+          <t>Tbl_DepartmentNames</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="0">
-        <v>569</v>
+        <v>731</v>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Tbl_EmailAddresses</t>
+          <t>Tbl_DocumentsToBeErased</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="0">
-        <v>570</v>
+        <v>732</v>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Tbl_EmailSoftware</t>
+          <t>Tbl_EmailAddresses</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="0">
-        <v>571</v>
+        <v>733</v>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Tbl_GeneralChart</t>
+          <t>Tbl_EmailSoftware</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="0">
-        <v>572</v>
+        <v>734</v>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Tbl_HelpPages</t>
+          <t>Tbl_GeneralChart</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="0">
-        <v>573</v>
+        <v>735</v>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Historical_Statements</t>
+          <t>Tbl_HelpPages</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="0">
-        <v>574</v>
+        <v>736</v>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>Tbl_HistoricalCLsAndStatements</t>
+          <t>Tbl_Historical_Statements</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="0">
-        <v>575</v>
+        <v>737</v>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>Tbl_HoldTypesToBeConsideredForCreditCheckReleases</t>
+          <t>Tbl_HistoricalCLsAndStatements</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="0">
-        <v>576</v>
+        <v>738</v>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>Tbl_InvoiceAttachments</t>
+          <t>Tbl_HoldTypesToBeConsideredForCreditCheckReleases</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="0">
-        <v>577</v>
+        <v>739</v>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Invoices</t>
+          <t>Tbl_InvoiceAttachments</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="0">
-        <v>578</v>
+        <v>740</v>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Invoices_History</t>
+          <t>Tbl_Invoices</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="0">
-        <v>579</v>
+        <v>741</v>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Languages</t>
+          <t>Tbl_Invoices_History</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="0">
-        <v>580</v>
+        <v>742</v>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Link_Customer_Internal_Email_Address</t>
+          <t>Tbl_Languages</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="0">
-        <v>581</v>
+        <v>743</v>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>TBL_LinkTemplateEmailAddress</t>
+          <t>Tbl_Link_Customer_Internal_Email_Address</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="0">
-        <v>582</v>
+        <v>744</v>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>Tbl_LOGICollectionsManagementReport</t>
+          <t>TBL_LinkTemplateEmailAddress</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="0">
-        <v>583</v>
+        <v>745</v>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>Tbl_MonthEnd</t>
+          <t>Tbl_LOGICollectionsManagementReport</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="0">
-        <v>584</v>
+        <v>746</v>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>Tbl_NEWS</t>
+          <t>Tbl_MonthEnd</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="0">
-        <v>585</v>
+        <v>747</v>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>Tbl_PaymentData</t>
+          <t>Tbl_NEWS</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="0">
-        <v>586</v>
+        <v>748</v>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>Tbl_queries</t>
+          <t>Tbl_PaymentData</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="0">
-        <v>587</v>
+        <v>749</v>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>Tbl_RSS</t>
+          <t>Tbl_queries</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="0">
-        <v>588</v>
+        <v>750</v>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>Tbl_SmartActivities</t>
+          <t>Tbl_RSS</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="0">
-        <v>589</v>
+        <v>751</v>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Templates</t>
+          <t>Tbl_SmartActivities</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="0">
-        <v>590</v>
+        <v>752</v>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Timezones</t>
+          <t>Tbl_Templates</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="0">
-        <v>591</v>
+        <v>753</v>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Top5ComplainingCustomers</t>
+          <t>Tbl_Timezones</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="0">
-        <v>592</v>
+        <v>754</v>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Top5WorseCustomers</t>
+          <t>Tbl_Top5ComplainingCustomers</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="0">
-        <v>593</v>
+        <v>755</v>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Types</t>
+          <t>Tbl_Top5WorseCustomers</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="0">
-        <v>594</v>
+        <v>756</v>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>Tbl_Users</t>
+          <t>Tbl_Types</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="0">
-        <v>595</v>
+        <v>757</v>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>Tbl_WhoPaidYesterday</t>
+          <t>Tbl_Users</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="0">
-        <v>596</v>
+        <v>758</v>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>TblGeneral</t>
+          <t>Tbl_WhoPaidYesterday</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="0">
-        <v>597</v>
+        <v>759</v>
       </c>
       <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>TblGeneral</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="52">
+      <c r="A52" s="0">
+        <v>760</v>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
         <is>
           <t>TblMain</t>
         </is>

</xml_diff>